<commit_message>
修改函数calc_strike_curve_and_greeks strike_curve[k_list[i]] 改为 strike_curve.iloc[i]: 按整数index写入series，防止K一致时索引至两行值，导致后续写入失败
</commit_message>
<xml_diff>
--- a/data/summary.xlsx
+++ b/data/summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>0M</t>
   </si>
@@ -35,18 +35,15 @@
   </si>
   <si>
     <t>right</t>
-  </si>
-  <si>
-    <t>2021-07-09 09:00:00</t>
-  </si>
-  <si>
-    <t>2021-07-09 09:01:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -99,9 +96,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -467,85 +467,85 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
+      <c r="A4" s="2">
+        <v>43467</v>
       </c>
       <c r="B4">
-        <v>-0.8426323123781735</v>
+        <v>-0.03056031644949887</v>
       </c>
       <c r="C4">
-        <v>0.003044935331461532</v>
+        <v>0.009336083822868596</v>
       </c>
       <c r="D4">
-        <v>0.845677247709635</v>
+        <v>0.03989640027236746</v>
       </c>
       <c r="E4">
-        <v>-0.05611393338790115</v>
+        <v>0.007339653571375165</v>
       </c>
       <c r="F4">
-        <v>0.02657253779449839</v>
+        <v>0.003696668535151762</v>
       </c>
       <c r="G4">
-        <v>0.08268647118239955</v>
+        <v>-0.003642985036223402</v>
       </c>
       <c r="H4">
-        <v>-0.0812652502576544</v>
+        <v>-0.02324686710860826</v>
       </c>
       <c r="I4">
-        <v>0.02789942292194518</v>
+        <v>-0.0116229998037474</v>
       </c>
       <c r="J4">
-        <v>0.1091646731795996</v>
+        <v>0.01162386730486087</v>
       </c>
       <c r="K4">
-        <v>0.007365897185004055</v>
+        <v>-0.002351533235689906</v>
       </c>
       <c r="L4">
-        <v>0.02091828061107031</v>
+        <v>0.01895979495127779</v>
       </c>
       <c r="M4">
-        <v>0.01355238342606625</v>
+        <v>0.0213113281869677</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
+      <c r="A5" s="2">
+        <v>43468</v>
       </c>
       <c r="B5">
-        <v>-0.8426323123781735</v>
+        <v>-0.01437140681067996</v>
       </c>
       <c r="C5">
-        <v>0.003044935331461532</v>
+        <v>0.006029594950748981</v>
       </c>
       <c r="D5">
-        <v>0.845677247709635</v>
+        <v>0.02040100176142894</v>
       </c>
       <c r="E5">
-        <v>-0.05611393338790115</v>
+        <v>-0.002347481293098961</v>
       </c>
       <c r="F5">
-        <v>0.02657253779449839</v>
+        <v>-0.001114083980204146</v>
       </c>
       <c r="G5">
-        <v>0.08268647118239955</v>
+        <v>0.001233397312894815</v>
       </c>
       <c r="H5">
-        <v>-0.0812652502576544</v>
+        <v>-0.004463858392987965</v>
       </c>
       <c r="I5">
-        <v>0.02789942292194518</v>
+        <v>-0.002162501257339382</v>
       </c>
       <c r="J5">
-        <v>0.1091646731795996</v>
+        <v>0.002301357135648583</v>
       </c>
       <c r="K5">
-        <v>0.007365897185004055</v>
+        <v>-0.005054024448394552</v>
       </c>
       <c r="L5">
-        <v>0.02091828061107031</v>
+        <v>0.02374142432484177</v>
       </c>
       <c r="M5">
-        <v>0.01355238342606625</v>
+        <v>0.02879544877323632</v>
       </c>
     </row>
   </sheetData>

</xml_diff>